<commit_message>
delete lead test case included
</commit_message>
<xml_diff>
--- a/data/TC005.xlsx
+++ b/data/TC005.xlsx
@@ -16,17 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Firstname</t>
   </si>
   <si>
-    <t>ganesh</t>
-  </si>
-  <si>
-    <t>ravisankar</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -37,6 +31,9 @@
   </si>
   <si>
     <t>crmsfa</t>
+  </si>
+  <si>
+    <t>ravi</t>
   </si>
 </sst>
 </file>
@@ -398,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,10 +410,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -424,24 +421,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>